<commit_message>
t aufzeichnugn + lab doc
</commit_message>
<xml_diff>
--- a/PREM/Zeitaufzeichnungen/ZeitaufzeichnungSeptember.xlsx
+++ b/PREM/Zeitaufzeichnungen/ZeitaufzeichnungSeptember.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\GitHub\3DHIF\DBI\Zeitaufzeichnungen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Documents\GitHub\3DHIF\PREM\Zeitaufzeichnungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF87732-F36B-4225-BFFA-C5DDC983BAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1F17ED-41A6-4FF8-8994-BCC5F52CECE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1D8CD667-A7EF-4BFB-8417-310C3CB05619}"/>
   </bookViews>
@@ -85,10 +85,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -423,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92603408-C500-4ED2-8432-1BCBCFD84CD1}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,11 +438,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -456,11 +456,22 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>45908</v>
       </c>
       <c r="B3">
         <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>45912</v>
+      </c>
+      <c r="B4">
+        <v>75</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>